<commit_message>
Add introduction section to RAM document
</commit_message>
<xml_diff>
--- a/PM/Responsibility Assignment Matrix.xlsx
+++ b/PM/Responsibility Assignment Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Salsabeel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
   <si>
     <t>Responsibility Assignment Matrix</t>
   </si>
@@ -82,68 +82,121 @@
     <t>Assign roles of planning phase</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction:
+    <t>Task / Responsible</t>
+  </si>
+  <si>
+    <t>Ahmed</t>
+  </si>
+  <si>
+    <t>Alaa</t>
+  </si>
+  <si>
+    <t>Hassan</t>
+  </si>
+  <si>
+    <t>Khadija</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Salsabeel </t>
+  </si>
+  <si>
+    <t>Sondos</t>
+  </si>
+  <si>
+    <t>Configuration management tool</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Risk Sheet</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Issues Sheet</t>
+  </si>
+  <si>
+    <t>Software Requirements Specification (SRS)</t>
+  </si>
+  <si>
+    <t>SRS Peer Review Sheet</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Requiremets Traceablity matrix (RTM)</t>
+  </si>
+  <si>
+    <t>SIQ</t>
+  </si>
+  <si>
+    <t>Project Plan Document</t>
+  </si>
+  <si>
+    <t>Project Schedule</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Introduction:
 </t>
-  </si>
-  <si>
-    <t>Task / Responsible</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>Alaa</t>
-  </si>
-  <si>
-    <t>Hassan</t>
-  </si>
-  <si>
-    <t>Khadija</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salsabeel </t>
-  </si>
-  <si>
-    <t>Sondos</t>
-  </si>
-  <si>
-    <t>Configuration management tool</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>Risk Sheet</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>Issues Sheet</t>
-  </si>
-  <si>
-    <t>Software Requirements Specification (SRS)</t>
-  </si>
-  <si>
-    <t>SRS Peer Review Sheet</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Requiremets Traceablity matrix (RTM)</t>
-  </si>
-  <si>
-    <t>SIQ</t>
-  </si>
-  <si>
-    <t>Project Plan Document</t>
-  </si>
-  <si>
-    <t>Project Schedule</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">A responsibility assignment Matrix (RAM), also known as RACI matrix, describes the participation by various roles in completing tasks or deliverables for a project or business process. It is used for clarifying and defining roles and responsibilities in cross-functional or departmental projects and processes.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>It defines four roles:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">R = Responsible (also Recommender)
+A = Accountable (also Approver or final approving authority)
+C = Consulted (sometimes Consultant or counsel)
+I = Informed (also Informee)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Add Introduction Section</t>
   </si>
 </sst>
 </file>
@@ -239,7 +292,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -514,142 +567,211 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -932,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -946,423 +1068,445 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="A2" s="39"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="A3" s="39"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="A5" s="39"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
+      <c r="J5" s="39"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="39"/>
     </row>
     <row r="7" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
+      <c r="A7" s="1"/>
+      <c r="B7" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="2"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="40"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="5" t="s">
+      <c r="F8" s="41"/>
+      <c r="G8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="7"/>
+      <c r="J8" s="42"/>
     </row>
     <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="5">
         <v>1</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="13"/>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="17"/>
-    </row>
-    <row r="13" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="18" t="s">
+      <c r="F9" s="43"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="43"/>
+      <c r="J9" s="44"/>
+    </row>
+    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B10" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="46">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D10" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="50"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="8"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="37"/>
+    </row>
+    <row r="14" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B15" s="38"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
+      <c r="I16" s="38"/>
+      <c r="J16" s="38"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B17" s="38"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="38"/>
+      <c r="J17" s="38"/>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B18" s="38"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
+      <c r="I19" s="38"/>
+      <c r="J19" s="38"/>
+    </row>
+    <row r="20" spans="2:10" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="38"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+    </row>
+    <row r="21" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="38"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+    </row>
+    <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="23" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="18"/>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
-      <c r="I14" s="18"/>
-      <c r="J14" s="18"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="18"/>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="18"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="18"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="18"/>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="18"/>
-      <c r="G18" s="18"/>
-      <c r="H18" s="18"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="18"/>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
-      <c r="F19" s="18"/>
-      <c r="G19" s="18"/>
-      <c r="H19" s="18"/>
-      <c r="I19" s="18"/>
-      <c r="J19" s="18"/>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="18"/>
-      <c r="G20" s="18"/>
-      <c r="H20" s="18"/>
-      <c r="I20" s="18"/>
-      <c r="J20" s="18"/>
-    </row>
-    <row r="21" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="22" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C22" s="19" t="s">
+      <c r="D23" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="E23" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="F23" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F22" s="21" t="s">
+      <c r="G23" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="H23" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="21" t="s">
+      <c r="I23" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I22" s="22" t="s">
+    </row>
+    <row r="24" spans="2:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C24" s="14" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="C23" s="23" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25" t="s">
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="27" t="s">
+      <c r="I24" s="19"/>
+    </row>
+    <row r="25" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C25" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="28"/>
-    </row>
-    <row r="24" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="C24" s="29" t="s">
+      <c r="D25" s="21"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="22"/>
+      <c r="H25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G24" s="31"/>
-      <c r="H24" s="33" t="s">
+    </row>
+    <row r="26" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C26" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="21"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I24" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="C25" s="29" t="s">
+      <c r="G26" s="22"/>
+      <c r="H26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="C27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="31"/>
-      <c r="F25" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="33" t="s">
+      <c r="D27" s="21"/>
+      <c r="E27" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I25" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="C26" s="29" t="s">
+      <c r="F27" s="22"/>
+      <c r="G27" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="22"/>
+      <c r="I27" s="27"/>
+    </row>
+    <row r="28" spans="2:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="30"/>
-      <c r="E26" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="31"/>
-      <c r="G26" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="31"/>
-      <c r="I26" s="36"/>
-    </row>
-    <row r="27" spans="2:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="C27" s="29" t="s">
+      <c r="D28" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="22"/>
+      <c r="F28" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="D27" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" s="31"/>
-      <c r="F27" s="38" t="s">
+      <c r="G28" s="22"/>
+      <c r="H28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="C29" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="31"/>
-      <c r="H27" s="33" t="s">
+      <c r="D29" s="21"/>
+      <c r="E29" s="22"/>
+      <c r="F29" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="22"/>
+      <c r="H29" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I29" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="C28" s="29" t="s">
+    </row>
+    <row r="30" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C30" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G28" s="31"/>
-      <c r="H28" s="33" t="s">
+      <c r="D30" s="21"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="I28" s="39" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="C29" s="29" t="s">
+      <c r="H30" s="22"/>
+      <c r="I30" s="25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C31" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="D29" s="30"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="32" t="s">
-        <v>22</v>
-      </c>
-      <c r="H29" s="31"/>
-      <c r="I29" s="34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="C30" s="29" t="s">
+      <c r="D31" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="F31" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="22"/>
+      <c r="H31" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I31" s="27"/>
+    </row>
+    <row r="32" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="37" t="s">
-        <v>22</v>
-      </c>
-      <c r="E30" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F30" s="35" t="s">
-        <v>24</v>
-      </c>
-      <c r="G30" s="31"/>
-      <c r="H30" s="33" t="s">
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I32" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="I30" s="36"/>
-    </row>
-    <row r="31" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C31" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D31" s="41"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
-      <c r="G31" s="42"/>
-      <c r="H31" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="44" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B13:J20"/>
+  <mergeCells count="11">
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B14:J21"/>
     <mergeCell ref="A1:J6"/>
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="I9:J9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add design phase roles
</commit_message>
<xml_diff>
--- a/PM/Responsibility Assignment Matrix.xlsx
+++ b/PM/Responsibility Assignment Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t>Responsibility Assignment Matrix</t>
   </si>
@@ -62,15 +62,6 @@
   </si>
   <si>
     <t>Comment</t>
-  </si>
-  <si>
-    <t>Peer Review</t>
-  </si>
-  <si>
-    <t>Peer Review Date</t>
-  </si>
-  <si>
-    <t>Peer Review comment</t>
   </si>
   <si>
     <t>Salsabeel</t>
@@ -201,6 +192,39 @@
   <si>
     <t xml:space="preserve">Update Roles </t>
   </si>
+  <si>
+    <t>Add roles for design tasks</t>
+  </si>
+  <si>
+    <t>Update project plan</t>
+  </si>
+  <si>
+    <t>GUI design</t>
+  </si>
+  <si>
+    <t>High level design</t>
+  </si>
+  <si>
+    <t>Desgin Data Models</t>
+  </si>
+  <si>
+    <t>Design class diagram</t>
+  </si>
+  <si>
+    <t>Write design document</t>
+  </si>
+  <si>
+    <t>Write design document peer review sheet</t>
+  </si>
+  <si>
+    <t>Design phase tasks</t>
+  </si>
+  <si>
+    <t>update RTM</t>
+  </si>
+  <si>
+    <t>Update RACI matrix</t>
+  </si>
 </sst>
 </file>
 
@@ -209,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,6 +286,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -301,7 +333,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -424,21 +456,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -549,21 +566,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -661,6 +663,91 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -669,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -686,101 +773,107 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -791,59 +884,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1125,10 +1220,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C15" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1138,448 +1233,613 @@
     <col min="7" max="10" width="20.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-    </row>
-    <row r="7" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="41"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="41"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="41"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="41"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+    </row>
+    <row r="7" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="F8" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="G8" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="41"/>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="50"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+    </row>
+    <row r="9" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="G9" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="42"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="43"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="44"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="35">
+      <c r="H9" s="52"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="47"/>
+    </row>
+    <row r="10" spans="1:11" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C10" s="53"/>
+      <c r="D10" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="28">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D10" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="37"/>
-      <c r="H10" s="37"/>
-      <c r="I10" s="45"/>
-      <c r="J10" s="47"/>
-    </row>
-    <row r="11" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="57">
+      <c r="F10" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="43" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="47"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C11" s="53"/>
+      <c r="D11" s="57" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="55">
         <v>2</v>
       </c>
-      <c r="D11" s="58">
+      <c r="F11" s="56">
         <v>43501</v>
       </c>
-      <c r="E11" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="56"/>
-    </row>
-    <row r="14" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="38" t="s">
+      <c r="G11" s="54" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="58"/>
+      <c r="I11" s="49"/>
+      <c r="J11" s="49"/>
+      <c r="K11" s="47"/>
+    </row>
+    <row r="12" spans="1:11" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="53"/>
+      <c r="D12" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="37">
+        <v>3</v>
+      </c>
+      <c r="F12" s="59">
+        <v>43713</v>
+      </c>
+      <c r="G12" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="H12" s="39"/>
+    </row>
+    <row r="14" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40"/>
+      <c r="E17" s="40"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" spans="2:10" ht="31.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" spans="2:10" ht="63" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="40"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
     </row>
     <row r="22" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="23" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="G23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="H23" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="I23" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="10" t="s">
+    </row>
+    <row r="24" spans="2:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C24" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="H23" s="10" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="F24" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="14" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="C24" s="12" t="s">
+      <c r="I24" s="15"/>
+    </row>
+    <row r="25" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="13"/>
-      <c r="E24" s="14" t="s">
+      <c r="D25" s="17"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F24" s="23" t="s">
+      <c r="H25" s="33"/>
+      <c r="I25" s="34"/>
+    </row>
+    <row r="26" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C26" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="17"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="33"/>
+      <c r="I26" s="34"/>
+    </row>
+    <row r="27" spans="2:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="C27" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="17"/>
+      <c r="E27" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="18"/>
+      <c r="G27" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="H27" s="18"/>
+      <c r="I27" s="23"/>
+    </row>
+    <row r="28" spans="2:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C28" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="G24" s="15"/>
-      <c r="H24" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I24" s="17"/>
-    </row>
-    <row r="25" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="C25" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-    </row>
-    <row r="26" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="C26" s="18" t="s">
+      <c r="D28" s="32"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-    </row>
-    <row r="27" spans="2:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="C27" s="18" t="s">
+      <c r="G28" s="18"/>
+      <c r="H28" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="54" x14ac:dyDescent="0.3">
+      <c r="C29" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="19"/>
-      <c r="E27" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="20"/>
-      <c r="I27" s="25"/>
-    </row>
-    <row r="28" spans="2:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="C28" s="18" t="s">
+      <c r="D29" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="E29" s="17"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D28" s="48"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="27" t="s">
+      <c r="D30" s="17"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="18"/>
+      <c r="I30" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="36" x14ac:dyDescent="0.3">
+      <c r="C31" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="54" x14ac:dyDescent="0.3">
-      <c r="C29" s="18" t="s">
+      <c r="D31" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="2:10" ht="18" x14ac:dyDescent="0.3">
+      <c r="C32" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="51" t="s">
-        <v>23</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="22" t="s">
+      <c r="D32" s="32"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="33"/>
+      <c r="H32" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I29" s="28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="18" x14ac:dyDescent="0.3">
-      <c r="C30" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="H30" s="20"/>
-      <c r="I30" s="23" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="36" x14ac:dyDescent="0.3">
-      <c r="C31" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="G31" s="20"/>
-      <c r="H31" s="22" t="s">
+      <c r="I32" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="60" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="62"/>
+    </row>
+    <row r="34" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C34" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="32"/>
+      <c r="E34" s="33"/>
+      <c r="F34" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="33"/>
+      <c r="H34" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="I31" s="25"/>
-    </row>
-    <row r="32" spans="2:10" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="30"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="I32" s="33" t="s">
-        <v>21</v>
-      </c>
+      <c r="I34" s="34"/>
+    </row>
+    <row r="35" spans="3:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="C35" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D35" s="32"/>
+      <c r="E35" s="33"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="34"/>
+    </row>
+    <row r="36" spans="3:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="C36" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D36" s="32"/>
+      <c r="E36" s="33"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" s="34"/>
+    </row>
+    <row r="37" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C37" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="33"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C38" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D38" s="32"/>
+      <c r="E38" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="34"/>
+    </row>
+    <row r="39" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C39" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="32"/>
+      <c r="E39" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="34"/>
+    </row>
+    <row r="40" spans="3:9" ht="54" x14ac:dyDescent="0.3">
+      <c r="C40" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="33"/>
+      <c r="F40" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="34"/>
+    </row>
+    <row r="41" spans="3:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="C41" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D41" s="32"/>
+      <c r="E41" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" s="33"/>
+      <c r="G41" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="33"/>
+      <c r="I41" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" ht="36" x14ac:dyDescent="0.3">
+      <c r="C42" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D42" s="32"/>
+      <c r="E42" s="33"/>
+      <c r="F42" s="33"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="I42" s="34"/>
+    </row>
+    <row r="43" spans="3:9" ht="18" x14ac:dyDescent="0.3">
+      <c r="C43" s="16"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="33"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="33"/>
+      <c r="H43" s="33"/>
+      <c r="I43" s="34"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="E11:F11"/>
+  <mergeCells count="13">
+    <mergeCell ref="C33:I33"/>
     <mergeCell ref="I11:J11"/>
     <mergeCell ref="B14:J21"/>
     <mergeCell ref="A1:J6"/>
     <mergeCell ref="B7:I7"/>
-    <mergeCell ref="E8:F8"/>
     <mergeCell ref="I8:J8"/>
-    <mergeCell ref="E9:F9"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E10:F10"/>
     <mergeCell ref="I10:J10"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>